<commit_message>
MAJ des exemples d4443d46afad24c2b9e6fb717d3a6120c0673f8f
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/StructureDefinition-SubmissionSet.xlsx
+++ b/add-info-dmp/ig/StructureDefinition-SubmissionSet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="118">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-03T14:02:53+00:00</t>
+    <t>2025-05-03T14:33:40+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -264,84 +264,88 @@
     <t>SubmissionSet.availabilityStatus</t>
   </si>
   <si>
+    <t xml:space="preserve">code
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette métadonnée représente la pertinence d'un lot de soumission. </t>
+  </si>
+  <si>
+    <t>Cette métadonnée représente la pertinence d'un lot de soumission.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'urn:oasis:names:tc:ebxml-regrep:StatusType:Approved': version à jour du lot de soumission. 'urn:asip:ci-sis:2010:StatusType:Archived': version archivée du lot de soumission, dans le cas où toutes les fiches du lot ont leur métadonnée availabilityStatus prenant la valeur  'urn:asip:ci-sis:2010:StatusType:Archived'. </t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>https://mos.esante.gouv.fr/NOS/JDV_J52-AvailabilityStatus-CISIS/FHIR/JDV-J52-AvailabilityStatus-CISIS</t>
+  </si>
+  <si>
+    <t>SubmissionSet.submissionTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dateTime
+</t>
+  </si>
+  <si>
+    <t>Représente la date et heure de soumission.</t>
+  </si>
+  <si>
+    <t>SubmissionSet.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titre du lot de soumission </t>
+  </si>
+  <si>
+    <t>Titre du lot de soumission</t>
+  </si>
+  <si>
+    <t>SubmissionSet.comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette métadonnée contient le commentaire associé au lot de soumission. </t>
+  </si>
+  <si>
+    <t>Cette métadonnée contient le commentaire associé au lot de soumission.</t>
+  </si>
+  <si>
+    <t>SubmissionSet.patientID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/PatientId
+</t>
+  </si>
+  <si>
+    <t>Cette métadonnée représente l’identifiant du patient, en l’occurrence, le matricule INS (NIR ou NIA) du patient tel que défini dans le cadre juridique.</t>
+  </si>
+  <si>
+    <t>SubmissionSet.sourceID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oid
+</t>
+  </si>
+  <si>
+    <t>Cette métadonnée représente l’identifiant unique global du système émetteur du lot de soumission</t>
+  </si>
+  <si>
+    <t>SubmissionSet.uniqueID</t>
+  </si>
+  <si>
+    <t>Identifiant unique global affecté à ce lot de soumission par son créateur. Cet attribut est utilisé à des fins de référence externe alors que entryUUID est destiné à des fins de gestion interne.</t>
+  </si>
+  <si>
+    <t>SubmissionSet.contentTypeCode</t>
+  </si>
+  <si>
     <t xml:space="preserve">CodeableConcept
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cette métadonnée représente la pertinence d'un lot de soumission. </t>
-  </si>
-  <si>
-    <t>Cette métadonnée représente la pertinence d'un lot de soumission.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'urn:oasis:names:tc:ebxml-regrep:StatusType:Approved': version à jour du lot de soumission. 'urn:asip:ci-sis:2010:StatusType:Archived': version archivée du lot de soumission, dans le cas où toutes les fiches du lot ont leur métadonnée availabilityStatus prenant la valeur  'urn:asip:ci-sis:2010:StatusType:Archived'. </t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>https://mos.esante.gouv.fr/NOS/JDV_J52-AvailabilityStatus-CISIS/FHIR/JDV-J52-AvailabilityStatus-CISIS</t>
-  </si>
-  <si>
-    <t>SubmissionSet.submissionTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dateTime
-</t>
-  </si>
-  <si>
-    <t>Représente la date et heure de soumission.</t>
-  </si>
-  <si>
-    <t>SubmissionSet.title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Titre du lot de soumission </t>
-  </si>
-  <si>
-    <t>Titre du lot de soumission</t>
-  </si>
-  <si>
-    <t>SubmissionSet.comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cette métadonnée contient le commentaire associé au lot de soumission. </t>
-  </si>
-  <si>
-    <t>Cette métadonnée contient le commentaire associé au lot de soumission.</t>
-  </si>
-  <si>
-    <t>SubmissionSet.patientID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/PatientId
-</t>
-  </si>
-  <si>
-    <t>Cette métadonnée représente l’identifiant du patient, en l’occurrence, le matricule INS (NIR ou NIA) du patient tel que défini dans le cadre juridique.</t>
-  </si>
-  <si>
-    <t>SubmissionSet.sourceID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oid
-</t>
-  </si>
-  <si>
-    <t>Cette métadonnée représente l’identifiant unique global du système émetteur du lot de soumission</t>
-  </si>
-  <si>
-    <t>SubmissionSet.uniqueID</t>
-  </si>
-  <si>
-    <t>Identifiant unique global affecté à ce lot de soumission par son créateur. Cet attribut est utilisé à des fins de référence externe alors que entryUUID est destiné à des fins de gestion interne.</t>
-  </si>
-  <si>
-    <t>SubmissionSet.contentTypeCode</t>
   </si>
   <si>
     <t xml:space="preserve">Ensemble de métadonnées représentant le type d’activité associé à l’événement clinique ayant abouti à la constitution du lot de soumission. </t>
@@ -1759,13 +1763,13 @@
         <v>72</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1796,7 +1800,7 @@
       </c>
       <c r="Y11" s="2"/>
       <c r="Z11" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AA11" t="s" s="2">
         <v>72</v>
@@ -1831,10 +1835,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -1857,13 +1861,13 @@
         <v>72</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -1914,7 +1918,7 @@
         <v>72</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>78</v>
@@ -1931,10 +1935,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -1960,10 +1964,10 @@
         <v>102</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -2014,7 +2018,7 @@
         <v>72</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>73</v>
@@ -2031,10 +2035,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -2060,10 +2064,10 @@
         <v>92</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -2114,7 +2118,7 @@
         <v>72</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>73</v>

</xml_diff>

<commit_message>
MAJ du lot de soummission 2c6aaa57e2c2acbc50515dd09f17f12486bbaa95
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/StructureDefinition-SubmissionSet.xlsx
+++ b/add-info-dmp/ig/StructureDefinition-SubmissionSet.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-03T15:10:00+00:00</t>
+    <t>2025-05-03T15:16:04+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -274,7 +274,7 @@
     <t>Cette métadonnée représente la pertinence d'un lot de soumission.</t>
   </si>
   <si>
-    <t xml:space="preserve">'urn:oasis:names:tc:ebxml-regrep:StatusType:Approved': version à jour du lot de soumission. 'urn:asip:ci-sis:2010:StatusType:Archived': version archivée du lot de soumission, dans le cas où toutes les fiches du lot ont leur métadonnée availabilityStatus prenant la valeur  'urn:asip:ci-sis:2010:StatusType:Archived'. </t>
+    <t xml:space="preserve">'urn:asip:ci-sis:2010:StatusType:Archived </t>
   </si>
   <si>
     <t>required</t>
@@ -709,7 +709,7 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="249.7109375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="34.046875" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>

</xml_diff>